<commit_message>
changed : move more in front and consolidate column date and time ago
</commit_message>
<xml_diff>
--- a/public/data/db_source/folder.xlsx
+++ b/public/data/db_source/folder.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1628B-311C-6348-B875-505A77AE2082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DE6784-8909-C54B-95FE-2E06F61C4B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,10 +781,10 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U25" sqref="U25"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1144,6 +1144,9 @@
       <c r="F15" t="s">
         <v>81</v>
       </c>
+      <c r="G15">
+        <v>2020</v>
+      </c>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>